<commit_message>
Update structure and diagram
</commit_message>
<xml_diff>
--- a/Document/Member.xlsx
+++ b/Document/Member.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VPS-Monitor\Teamwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IMS-datacenter\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20340" windowHeight="7875"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20340" windowHeight="7875" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Taido" sheetId="2" r:id="rId2"/>
+    <sheet name="Budget" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Lê Thị Thu Hà</t>
     <phoneticPr fontId="1"/>
@@ -194,12 +194,33 @@
   <si>
     <t>thời gian nhóm gặp chủ yếu là từ: slot 2+3 hoặc 4+5+6</t>
   </si>
+  <si>
+    <t>Trước đó</t>
+  </si>
+  <si>
+    <t>Chi tiêu</t>
+  </si>
+  <si>
+    <t>Nội dung</t>
+  </si>
+  <si>
+    <t>Quỹ</t>
+  </si>
+  <si>
+    <t>Mỗi người đóng 100k</t>
+  </si>
+  <si>
+    <t>Đi uống với anh Mạnh hỏi về đồ án</t>
+  </si>
+  <si>
+    <t>Đi uống với anh Tùng, nhờ anh chỉ về code nền tảng</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +279,15 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -395,7 +425,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -456,7 +486,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -939,7 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -954,22 +990,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="18">
       <c r="A4" s="1" t="s">
@@ -1125,7 +1161,7 @@
   <dimension ref="A4:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1201,13 +1237,69 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" ht="15">
+      <c r="B3" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="20"/>
+      <c r="C5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="20">
+        <v>42384</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="8">
+        <v>300</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update GUI & assign task
</commit_message>
<xml_diff>
--- a/Document/Member.xlsx
+++ b/Document/Member.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IMS-datacenter\DOCUMENT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new place\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20340" windowHeight="7875" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20340" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Chú ý" sheetId="2" r:id="rId2"/>
     <sheet name="Budget" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Lê Thị Thu Hà</t>
     <phoneticPr fontId="1"/>
@@ -235,23 +235,29 @@
   <si>
     <t>Tổng</t>
   </si>
+  <si>
+    <t>Bánh mì và nước ở the coffeehouse đợt 1</t>
+  </si>
+  <si>
+    <t>Bánh mì và nước ở the coffeehouse đợt 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -260,7 +266,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -303,7 +309,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -524,10 +530,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1013,37 +1019,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="3" width="19.75" style="2" customWidth="1"/>
-    <col min="4" max="5" width="13.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.75" style="2" customWidth="1"/>
+    <col min="2" max="3" width="19.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="4" spans="1:7" ht="18">
       <c r="A4" s="1" t="s">
@@ -1202,11 +1208,11 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="62.25" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:4" s="18" customFormat="1">
@@ -1237,7 +1243,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="114">
+    <row r="6" spans="1:4" ht="120">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -1281,20 +1287,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F13"/>
+  <dimension ref="B3:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.75" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15">
+    <row r="3" spans="2:6">
       <c r="B3" s="21" t="s">
         <v>31</v>
       </c>
@@ -1307,7 +1313,7 @@
       <c r="E3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="20" t="s">
@@ -1380,40 +1386,58 @@
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="8">
+        <v>300</v>
+      </c>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="8">
-        <f>SUM(D4:D12)</f>
-        <v>300</v>
-      </c>
-      <c r="E13" s="8">
-        <f>SUM(E4:E12)</f>
-        <v>283</v>
+      <c r="C14" s="25"/>
+      <c r="D14" s="8">
+        <f>SUM(D4:D13)</f>
+        <v>600</v>
+      </c>
+      <c r="E14" s="8">
+        <f>SUM(E4:E13)</f>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update data add server
</commit_message>
<xml_diff>
--- a/Document/Member.xlsx
+++ b/Document/Member.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20340" windowHeight="7875"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20340" windowHeight="7875" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Lê Thị Thu Hà</t>
     <phoneticPr fontId="1"/>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>Bánh mì và nước ở the coffeehouse đợt 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ăn kem </t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1289,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1416,10 +1419,16 @@
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="20">
+        <v>42454</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="25" t="s">
@@ -1432,7 +1441,7 @@
       </c>
       <c r="E14" s="8">
         <f>SUM(E4:E13)</f>
-        <v>416</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test list + add Q&A
</commit_message>
<xml_diff>
--- a/Document/Member.xlsx
+++ b/Document/Member.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Lê Thị Thu Hà</t>
     <phoneticPr fontId="1"/>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>Uống nước với anh mạnh ở mộc high-end</t>
+  </si>
+  <si>
+    <t>In thử bản 38tr. Kẹp lò xo 15k, 3 tờ A3 12k, 35 tờ A4 màu 35k</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1305,7 @@
   <dimension ref="B3:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1490,10 +1493,16 @@
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="20"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="20">
+        <v>42473</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8">
+        <v>62</v>
+      </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="20"/>
@@ -1517,8 +1526,8 @@
         <v>600</v>
       </c>
       <c r="E21" s="8">
-        <f>SUM(E4:E17)</f>
-        <v>806</v>
+        <f>SUM(E4:E18)</f>
+        <v>868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update code + presentation
</commit_message>
<xml_diff>
--- a/Document/Member.xlsx
+++ b/Document/Member.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>Lê Thị Thu Hà</t>
     <phoneticPr fontId="1"/>
@@ -255,6 +255,18 @@
   </si>
   <si>
     <t>In thử bản 38tr. Kẹp lò xo 15k, 3 tờ A3 12k, 35 tờ A4 màu 35k</t>
+  </si>
+  <si>
+    <t>In bản chính thức. 5 bộ 200tr, 5 bộ 38tr</t>
+  </si>
+  <si>
+    <t>Uống nước tại Moda</t>
+  </si>
+  <si>
+    <t>Ăn trưa mì xào bò 3 hộp</t>
+  </si>
+  <si>
+    <t>Mua bánh mì cho anh Tùng</t>
   </si>
 </sst>
 </file>
@@ -1302,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F21"/>
+  <dimension ref="B3:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E23" sqref="B23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1505,34 +1517,82 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="20"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="20">
+        <v>42475</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8">
+        <v>780</v>
+      </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="20"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="20">
+        <v>42475</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8">
+        <v>76</v>
+      </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="20">
+        <v>42109</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="20">
+        <v>42475</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="20"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="20"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="8">
+      <c r="C25" s="25"/>
+      <c r="D25" s="8">
         <f>SUM(D4:D14)</f>
         <v>600</v>
       </c>
-      <c r="E21" s="8">
-        <f>SUM(E4:E18)</f>
-        <v>868</v>
+      <c r="E25" s="8">
+        <f>SUM(E4:E24)</f>
+        <v>1809</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>